<commit_message>
Some hyperlinks added to examples of previous year repos.
</commit_message>
<xml_diff>
--- a/Examples/Repos_2017_2018.xlsx
+++ b/Examples/Repos_2017_2018.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/cas741/Examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71FF204-3D87-D44B-BDF3-331D30819FD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="1720" windowWidth="47520" windowHeight="21560" tabRatio="500"/>
+    <workbookView xWindow="1580" yWindow="1720" windowWidth="47520" windowHeight="21560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -143,7 +144,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -236,7 +237,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -260,8 +261,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -271,8 +273,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="23"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="24">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -295,6 +298,7 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -302,6 +306,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -569,11 +576,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -821,7 +828,7 @@
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>17</v>
       </c>
       <c r="H9" t="s">
@@ -852,7 +859,7 @@
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
       <c r="H10" t="s">
@@ -914,7 +921,7 @@
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H12" t="s">
@@ -1005,6 +1012,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{AF21CDB9-AA3D-3D48-876F-25B3BDF21728}"/>
+    <hyperlink ref="B10" r:id="rId2" xr:uid="{122A7680-49F4-4342-82E2-81736E970A2F}"/>
+    <hyperlink ref="B12" r:id="rId3" xr:uid="{18A0A668-C44B-5D4C-9E82-6E927828576D}"/>
+  </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>

</xml_diff>